<commit_message>
Site updated: 2024-05-05 16:24:16
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -508,13 +508,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -542,13 +542,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -576,13 +576,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -610,13 +610,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -644,13 +644,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -678,13 +678,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -712,13 +712,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -814,13 +814,13 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -848,13 +848,13 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -882,13 +882,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -916,13 +916,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -950,13 +950,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -984,13 +984,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1018,13 +1018,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1052,13 +1052,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1222,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1256,13 +1256,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1290,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1324,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1698,13 +1698,13 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1902,13 +1902,13 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1942,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -2004,13 +2004,13 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -2140,13 +2140,13 @@
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -2174,13 +2174,13 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -2208,13 +2208,13 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2276,13 +2276,13 @@
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -2310,13 +2310,13 @@
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2412,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2443,16 +2443,16 @@
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -2511,16 +2511,16 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -2545,16 +2545,16 @@
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2579,10 +2579,10 @@
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -2613,16 +2613,16 @@
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2647,16 +2647,16 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2681,16 +2681,16 @@
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2715,16 +2715,16 @@
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2749,16 +2749,16 @@
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2783,16 +2783,16 @@
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -2851,16 +2851,16 @@
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2885,16 +2885,16 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2919,16 +2919,16 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -2953,16 +2953,16 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2987,16 +2987,16 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -3021,16 +3021,16 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -3055,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -3089,16 +3089,16 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -3123,16 +3123,16 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -3157,16 +3157,16 @@
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -3191,16 +3191,16 @@
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -3225,16 +3225,16 @@
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -3259,16 +3259,16 @@
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -3293,10 +3293,10 @@
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -3327,10 +3327,10 @@
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -3361,16 +3361,16 @@
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -3395,16 +3395,16 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -3429,16 +3429,16 @@
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" t="n">
         <v>0</v>
@@ -3463,16 +3463,16 @@
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -3497,16 +3497,16 @@
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H90" t="n">
         <v>0</v>
@@ -3531,10 +3531,10 @@
         <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -3565,16 +3565,16 @@
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3599,16 +3599,16 @@
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93" t="n">
         <v>0</v>
@@ -3633,16 +3633,16 @@
         <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -3667,16 +3667,16 @@
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3701,10 +3701,10 @@
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -3735,16 +3735,16 @@
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H97" t="n">
         <v>0</v>
@@ -3769,16 +3769,16 @@
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" t="n">
         <v>0</v>
@@ -3803,16 +3803,16 @@
         <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -3837,10 +3837,10 @@
         <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -3871,16 +3871,16 @@
         <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H101" t="n">
         <v>0</v>
@@ -3905,10 +3905,10 @@
         <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -3939,10 +3939,10 @@
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
@@ -3973,10 +3973,10 @@
         <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -4007,16 +4007,16 @@
         <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" t="n">
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H105" t="n">
         <v>0</v>
@@ -4041,10 +4041,10 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" t="n">
         <v>0</v>
@@ -4075,10 +4075,10 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -4109,10 +4109,10 @@
         <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" t="n">
         <v>0</v>
@@ -4143,10 +4143,10 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" t="n">
         <v>0</v>
@@ -4177,10 +4177,10 @@
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" t="n">
         <v>0</v>
@@ -4211,10 +4211,10 @@
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" t="n">
         <v>0</v>
@@ -4245,16 +4245,16 @@
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" t="n">
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H112" t="n">
         <v>0</v>
@@ -4279,10 +4279,10 @@
         <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113" t="n">
         <v>0</v>
@@ -4313,10 +4313,10 @@
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F114" t="n">
         <v>0</v>
@@ -4347,10 +4347,10 @@
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115" t="n">
         <v>0</v>
@@ -4381,10 +4381,10 @@
         <v>0</v>
       </c>
       <c r="D116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" t="n">
         <v>0</v>
@@ -4415,10 +4415,10 @@
         <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F117" t="n">
         <v>0</v>
@@ -4449,10 +4449,10 @@
         <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F118" t="n">
         <v>0</v>
@@ -4486,13 +4486,13 @@
         <v>1</v>
       </c>
       <c r="E119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F119" t="n">
         <v>0</v>
       </c>
       <c r="G119" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H119" t="n">
         <v>0</v>
@@ -4520,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="E120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120" t="n">
         <v>0</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F121" t="n">
         <v>0</v>
@@ -4588,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
@@ -4622,7 +4622,7 @@
         <v>1</v>
       </c>
       <c r="E123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F123" t="n">
         <v>0</v>
@@ -4656,7 +4656,7 @@
         <v>1</v>
       </c>
       <c r="E124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F124" t="n">
         <v>0</v>
@@ -4690,7 +4690,7 @@
         <v>1</v>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F125" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-06 21:16:11
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4755,25 +4755,25 @@
         <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F127" t="n">
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H127" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -4789,25 +4789,25 @@
         <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H128" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">

</xml_diff>

<commit_message>
Site updated: 2024-05-07 22:06:01
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4820,28 +4820,28 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">

</xml_diff>

<commit_message>
Site updated: 2024-05-08 22:48:28
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4854,19 +4854,19 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H130" t="n">
         <v>0</v>
@@ -4875,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="J130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">

</xml_diff>

<commit_message>
Site updated: 2024-05-09 21:19:46
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4888,28 +4888,28 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H131" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I131" t="n">
         <v>0</v>
       </c>
       <c r="J131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">

</xml_diff>

<commit_message>
Site updated: 2024-05-10 11:24:42
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4922,13 +4922,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F132" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-10 23:42:44
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4931,13 +4931,13 @@
         <v>1</v>
       </c>
       <c r="F132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H132" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I132" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-11 23:54:33
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4956,13 +4956,13 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F133" t="n">
         <v>0</v>
@@ -4971,7 +4971,7 @@
         <v>0</v>
       </c>
       <c r="H133" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I133" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-12 22:08:06
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -4993,19 +4993,19 @@
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F134" t="n">
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I134" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-16 13:49:50
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5024,19 +5024,19 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135" t="n">
         <v>0</v>
       </c>
       <c r="G135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H135" t="n">
         <v>0</v>
@@ -5058,19 +5058,19 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136" t="n">
         <v>0</v>
       </c>
       <c r="G136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H136" t="n">
         <v>0</v>
@@ -5107,7 +5107,7 @@
         <v>0</v>
       </c>
       <c r="H137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I137" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-17 10:22:22
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5132,13 +5132,13 @@
         <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" t="n">
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H138" t="n">
         <v>0</v>
@@ -5147,7 +5147,7 @@
         <v>0</v>
       </c>
       <c r="J138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">

</xml_diff>

<commit_message>
Site updated: 2024-05-19 19:56:19
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5160,19 +5160,19 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" t="n">
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H139" t="n">
         <v>0</v>
@@ -5194,13 +5194,13 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F140" t="n">
         <v>0</v>
@@ -5228,19 +5228,19 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F141" t="n">
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-21 13:49:36
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5240,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H141" t="n">
         <v>0</v>
@@ -5268,7 +5268,7 @@
         <v>0</v>
       </c>
       <c r="E142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F142" t="n">
         <v>0</v>
@@ -5283,7 +5283,7 @@
         <v>0</v>
       </c>
       <c r="J142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">

</xml_diff>

<commit_message>
Site updated: 2024-05-22 22:43:18
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5302,19 +5302,19 @@
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F143" t="n">
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J143" t="n">
         <v>0</v>
@@ -5330,19 +5330,19 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H144" t="n">
         <v>0</v>
@@ -5351,7 +5351,7 @@
         <v>0</v>
       </c>
       <c r="J144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">

</xml_diff>

<commit_message>
Site updated: 2024-05-24 09:37:45
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5364,13 +5364,13 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -5379,7 +5379,7 @@
         <v>0</v>
       </c>
       <c r="H145" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I145" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-24 22:22:54
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5398,28 +5398,28 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
       </c>
       <c r="G146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">

</xml_diff>

<commit_message>
Site updated: 2024-05-25 11:28:26
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5379,7 +5379,7 @@
         <v>0</v>
       </c>
       <c r="H145" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I145" t="n">
         <v>0</v>
@@ -5413,7 +5413,7 @@
         <v>1</v>
       </c>
       <c r="H146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I146" t="n">
         <v>1</v>
@@ -5432,13 +5432,13 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F147" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-25 22:52:58
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5432,28 +5432,28 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H147" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I147" t="n">
         <v>0</v>
       </c>
       <c r="J147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">

</xml_diff>

<commit_message>
Site updated: 2024-05-26 22:31:34
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5466,28 +5466,28 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F148" t="n">
         <v>0</v>
       </c>
       <c r="G148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H148" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I148" t="n">
         <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">

</xml_diff>

<commit_message>
Site updated: 2024-05-28 10:28:47
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5500,22 +5500,22 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G149" t="n">
         <v>0</v>
       </c>
       <c r="H149" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I149" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-05-29 21:19:38
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5568,28 +5568,28 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H151" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I151" t="n">
         <v>0</v>
       </c>
       <c r="J151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">

</xml_diff>

<commit_message>
Site updated: 2024-06-01 23:22:44
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5602,19 +5602,19 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H152" t="n">
         <v>0</v>
@@ -5623,7 +5623,7 @@
         <v>0</v>
       </c>
       <c r="J152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -5636,16 +5636,16 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G153" t="n">
         <v>0</v>
@@ -5676,13 +5676,13 @@
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F154" t="n">
         <v>0</v>
       </c>
       <c r="G154" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H154" t="n">
         <v>0</v>
@@ -5691,7 +5691,7 @@
         <v>0</v>
       </c>
       <c r="J154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">

</xml_diff>

<commit_message>
Site updated: 2024-06-03 08:20:45
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5704,28 +5704,28 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J155" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">

</xml_diff>

<commit_message>
Site updated: 2024-06-03 22:34:13
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5738,28 +5738,28 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G156" t="n">
         <v>0</v>
       </c>
       <c r="H156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">

</xml_diff>

<commit_message>
Site updated: 2024-06-04 23:54:35
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5772,22 +5772,22 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G157" t="n">
         <v>0</v>
       </c>
       <c r="H157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I157" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-05 23:56:05
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5806,25 +5806,25 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F158" t="n">
         <v>0</v>
       </c>
       <c r="G158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H158" t="n">
         <v>0</v>
       </c>
       <c r="I158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J158" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-07 07:28:56
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5840,13 +5840,13 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F159" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-09 07:48:15
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5874,13 +5874,13 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F160" t="n">
         <v>0</v>
@@ -5908,19 +5908,19 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D161" t="n">
         <v>0</v>
       </c>
       <c r="E161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F161" t="n">
         <v>0</v>
       </c>
       <c r="G161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H161" t="n">
         <v>0</v>
@@ -5929,7 +5929,7 @@
         <v>0</v>
       </c>
       <c r="J161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">

</xml_diff>

<commit_message>
Site updated: 2024-06-09 23:14:53
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5942,10 +5942,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E162" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-11 09:38:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -5979,16 +5979,16 @@
         <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H163" t="n">
         <v>0</v>
@@ -5997,7 +5997,7 @@
         <v>0</v>
       </c>
       <c r="J163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">

</xml_diff>

<commit_message>
Site updated: 2024-06-17 22:43:45
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6214,28 +6214,28 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D170" t="n">
         <v>0</v>
       </c>
       <c r="E170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I170" t="n">
         <v>0</v>
       </c>
       <c r="J170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">

</xml_diff>

<commit_message>
Site updated: 2024-06-19 11:33:05
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6248,28 +6248,28 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
       </c>
       <c r="E171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F171" t="n">
         <v>0</v>
       </c>
       <c r="G171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H171" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I171" t="n">
         <v>0</v>
       </c>
       <c r="J171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">

</xml_diff>

<commit_message>
Site updated: 2024-06-19 22:42:48
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6282,28 +6282,28 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D172" t="n">
         <v>0</v>
       </c>
       <c r="E172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H172" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">

</xml_diff>

<commit_message>
Site updated: 2024-06-21 08:33:41
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6316,13 +6316,13 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D173" t="n">
         <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F173" t="n">
         <v>0</v>
@@ -6331,13 +6331,13 @@
         <v>0</v>
       </c>
       <c r="H173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I173" t="n">
         <v>0</v>
       </c>
       <c r="J173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">

</xml_diff>

<commit_message>
Site updated: 2024-06-22 08:33:03
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6356,16 +6356,16 @@
         <v>0</v>
       </c>
       <c r="E174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I174" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-22 23:35:35
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6390,16 +6390,16 @@
         <v>0</v>
       </c>
       <c r="E175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G175" t="n">
         <v>0</v>
       </c>
       <c r="H175" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I175" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-23 20:04:56
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6424,22 +6424,22 @@
         <v>0</v>
       </c>
       <c r="E176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G176" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H176" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I176" t="n">
         <v>0</v>
       </c>
       <c r="J176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">

</xml_diff>

<commit_message>
Site updated: 2024-06-24 23:13:24
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6452,28 +6452,28 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D177" t="n">
         <v>0</v>
       </c>
       <c r="E177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I177" t="n">
         <v>0</v>
       </c>
       <c r="J177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178">

</xml_diff>

<commit_message>
Site updated: 2024-06-25 23:19:11
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6486,19 +6486,19 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D178" t="n">
         <v>0</v>
       </c>
       <c r="E178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H178" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-27 00:00:09
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6520,28 +6520,28 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D179" t="n">
         <v>0</v>
       </c>
       <c r="E179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H179" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I179" t="n">
         <v>0</v>
       </c>
       <c r="J179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">

</xml_diff>

<commit_message>
Site updated: 2024-06-27 23:05:25
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6554,28 +6554,28 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D180" t="n">
         <v>0</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H180" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I180" t="n">
         <v>0</v>
       </c>
       <c r="J180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">

</xml_diff>

<commit_message>
Site updated: 2024-06-29 07:27:54
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6588,19 +6588,19 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D181" t="n">
         <v>0</v>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H181" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-06-30 00:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6622,28 +6622,28 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D182" t="n">
         <v>0</v>
       </c>
       <c r="E182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G182" t="n">
         <v>0</v>
       </c>
       <c r="H182" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I182" t="n">
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">

</xml_diff>

<commit_message>
Site updated: 2024-07-01 00:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6656,28 +6656,28 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D183" t="n">
         <v>0</v>
       </c>
       <c r="E183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G183" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H183" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I183" t="n">
         <v>0</v>
       </c>
       <c r="J183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">

</xml_diff>

<commit_message>
Site updated: 2024-07-01 23:56:23
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6690,19 +6690,19 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D184" t="n">
         <v>0</v>
       </c>
       <c r="E184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H184" t="n">
         <v>0</v>
@@ -6711,7 +6711,7 @@
         <v>0</v>
       </c>
       <c r="J184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">

</xml_diff>

<commit_message>
Site updated: 2024-07-03 00:00:06
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6724,19 +6724,19 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D185" t="n">
         <v>0</v>
       </c>
       <c r="E185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H185" t="n">
         <v>0</v>
@@ -6745,7 +6745,7 @@
         <v>0</v>
       </c>
       <c r="J185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">

</xml_diff>

<commit_message>
Site updated: 2024-07-04 00:00:42
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6758,19 +6758,19 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D186" t="n">
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H186" t="n">
         <v>0</v>
@@ -6779,7 +6779,7 @@
         <v>0</v>
       </c>
       <c r="J186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">

</xml_diff>

<commit_message>
Site updated: 2024-07-05 00:00:44
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6792,28 +6792,28 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D187" t="n">
         <v>0</v>
       </c>
       <c r="E187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I187" t="n">
         <v>0</v>
       </c>
       <c r="J187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">

</xml_diff>

<commit_message>
Site updated: 2024-07-06 00:00:48
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6826,19 +6826,19 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D188" t="n">
         <v>0</v>
       </c>
       <c r="E188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F188" t="n">
         <v>0</v>
       </c>
       <c r="G188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H188" t="n">
         <v>0</v>
@@ -6847,7 +6847,7 @@
         <v>0</v>
       </c>
       <c r="J188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">

</xml_diff>

<commit_message>
Site updated: 2024-07-06 23:42:01
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6860,28 +6860,28 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D189" t="n">
         <v>0</v>
       </c>
       <c r="E189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H189" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I189" t="n">
         <v>0</v>
       </c>
       <c r="J189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">

</xml_diff>

<commit_message>
Site updated: 2024-07-08 00:00:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6900,10 +6900,10 @@
         <v>0</v>
       </c>
       <c r="E190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G190" t="n">
         <v>0</v>
@@ -6915,7 +6915,7 @@
         <v>0</v>
       </c>
       <c r="J190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">

</xml_diff>

<commit_message>
Site updated: 2024-07-09 00:00:09
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6928,19 +6928,19 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D191" t="n">
         <v>0</v>
       </c>
       <c r="E191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F191" t="n">
         <v>0</v>
       </c>
       <c r="G191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H191" t="n">
         <v>0</v>
@@ -6949,7 +6949,7 @@
         <v>0</v>
       </c>
       <c r="J191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">

</xml_diff>

<commit_message>
Site updated: 2024-07-10 12:00:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6962,13 +6962,13 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D192" t="n">
         <v>0</v>
       </c>
       <c r="E192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F192" t="n">
         <v>0</v>
@@ -6983,7 +6983,7 @@
         <v>0</v>
       </c>
       <c r="J192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">

</xml_diff>

<commit_message>
Site updated: 2024-07-11 00:00:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -6999,25 +6999,25 @@
         <v>0</v>
       </c>
       <c r="D193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I193" t="n">
         <v>0</v>
       </c>
       <c r="J193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">

</xml_diff>

<commit_message>
Site updated: 2024-07-11 23:56:40
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7030,28 +7030,28 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">

</xml_diff>

<commit_message>
Site updated: 2024-07-13 00:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7064,28 +7064,28 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H195" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I195" t="n">
         <v>0</v>
       </c>
       <c r="J195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">

</xml_diff>

<commit_message>
Site updated: 2024-07-14 00:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7098,13 +7098,13 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D196" t="n">
         <v>0</v>
       </c>
       <c r="E196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F196" t="n">
         <v>0</v>
@@ -7113,7 +7113,7 @@
         <v>0</v>
       </c>
       <c r="H196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I196" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-07-15 12:00:10
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7138,10 +7138,10 @@
         <v>0</v>
       </c>
       <c r="E197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G197" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-07-16 00:00:13
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7172,10 +7172,10 @@
         <v>0</v>
       </c>
       <c r="E198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G198" t="n">
         <v>0</v>
@@ -7187,7 +7187,7 @@
         <v>0</v>
       </c>
       <c r="J198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">

</xml_diff>

<commit_message>
Site updated: 2024-07-18 00:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7200,13 +7200,13 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D199" t="n">
         <v>0</v>
       </c>
       <c r="E199" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F199" t="n">
         <v>0</v>
@@ -7240,10 +7240,10 @@
         <v>0</v>
       </c>
       <c r="E200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G200" t="n">
         <v>0</v>
@@ -7252,10 +7252,10 @@
         <v>0</v>
       </c>
       <c r="I200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">

</xml_diff>

<commit_message>
Site updated: 2024-07-19 00:00:05
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7268,19 +7268,19 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D201" t="n">
         <v>0</v>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H201" t="n">
         <v>0</v>
@@ -7289,7 +7289,7 @@
         <v>0</v>
       </c>
       <c r="J201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">

</xml_diff>

<commit_message>
Site updated: 2024-07-20 12:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7302,16 +7302,16 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D202" t="n">
         <v>0</v>
       </c>
       <c r="E202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G202" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-07-21 00:00:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7342,13 +7342,13 @@
         <v>0</v>
       </c>
       <c r="E203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F203" t="n">
         <v>0</v>
       </c>
       <c r="G203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H203" t="n">
         <v>0</v>
@@ -7357,7 +7357,7 @@
         <v>0</v>
       </c>
       <c r="J203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">

</xml_diff>

<commit_message>
Site updated: 2024-07-22 08:55:16
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7410,16 +7410,16 @@
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I205" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-07-23 00:00:06
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7410,7 +7410,7 @@
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F205" t="n">
         <v>1</v>
@@ -7419,7 +7419,7 @@
         <v>1</v>
       </c>
       <c r="H205" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I205" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-07-24 00:00:07
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7438,22 +7438,22 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D206" t="n">
         <v>0</v>
       </c>
       <c r="E206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G206" t="n">
         <v>0</v>
       </c>
       <c r="H206" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I206" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Site updated: 2024-07-25 00:00:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7478,13 +7478,13 @@
         <v>0</v>
       </c>
       <c r="E207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F207" t="n">
         <v>0</v>
       </c>
       <c r="G207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H207" t="n">
         <v>0</v>
@@ -7493,7 +7493,7 @@
         <v>0</v>
       </c>
       <c r="J207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208">

</xml_diff>

<commit_message>
Site updated: 2024-07-25 22:52:51
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7506,28 +7506,28 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D208" t="n">
         <v>0</v>
       </c>
       <c r="E208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H208" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I208" t="n">
         <v>0</v>
       </c>
       <c r="J208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">

</xml_diff>

<commit_message>
Site updated: 2024-07-27 16:41:49
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7540,28 +7540,28 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D209" t="n">
         <v>0</v>
       </c>
       <c r="E209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G209" t="n">
         <v>0</v>
       </c>
       <c r="H209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">

</xml_diff>

<commit_message>
Site updated: 2024-07-28 00:00:42
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7580,22 +7580,22 @@
         <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">

</xml_diff>

<commit_message>
Site updated: 2024-07-29 00:00:09
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7608,19 +7608,19 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D211" t="n">
         <v>0</v>
       </c>
       <c r="E211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H211" t="n">
         <v>0</v>
@@ -7629,7 +7629,7 @@
         <v>0</v>
       </c>
       <c r="J211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">

</xml_diff>

<commit_message>
Site updated: 2024-07-30 12:00:57
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7642,28 +7642,28 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D212" t="n">
         <v>0</v>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I212" t="n">
         <v>0</v>
       </c>
       <c r="J212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213">

</xml_diff>

<commit_message>
Site updated: 2024-07-31 07:35:45
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7682,10 +7682,10 @@
         <v>0</v>
       </c>
       <c r="E213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G213" t="n">
         <v>0</v>
@@ -7697,7 +7697,7 @@
         <v>0</v>
       </c>
       <c r="J213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214">

</xml_diff>

<commit_message>
Site updated: 2024-08-01 00:00:18
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7710,28 +7710,28 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D214" t="n">
         <v>0</v>
       </c>
       <c r="E214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H214" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I214" t="n">
         <v>0</v>
       </c>
       <c r="J214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">

</xml_diff>

<commit_message>
Site updated: 2024-08-02 00:00:51
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7744,28 +7744,28 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D215" t="n">
         <v>0</v>
       </c>
       <c r="E215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I215" t="n">
         <v>0</v>
       </c>
       <c r="J215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">

</xml_diff>

<commit_message>
Site updated: 2024-08-03 00:00:08
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7778,28 +7778,28 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D216" t="n">
         <v>0</v>
       </c>
       <c r="E216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G216" t="n">
         <v>0</v>
       </c>
       <c r="H216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I216" t="n">
         <v>0</v>
       </c>
       <c r="J216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">

</xml_diff>

<commit_message>
Site updated: 2024-08-04 07:25:17
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7812,19 +7812,19 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D217" t="n">
         <v>0</v>
       </c>
       <c r="E217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G217" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H217" t="n">
         <v>0</v>
@@ -7833,7 +7833,7 @@
         <v>0</v>
       </c>
       <c r="J217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">

</xml_diff>

<commit_message>
Site updated: 2024-08-06 06:00:57
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7880,19 +7880,19 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D219" t="n">
         <v>0</v>
       </c>
       <c r="E219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H219" t="n">
         <v>0</v>
@@ -7901,7 +7901,7 @@
         <v>0</v>
       </c>
       <c r="J219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">

</xml_diff>

<commit_message>
Site updated: 2024-08-07 21:21:40
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7914,16 +7914,16 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D220" t="n">
         <v>0</v>
       </c>
       <c r="E220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G220" t="n">
         <v>0</v>
@@ -7935,7 +7935,7 @@
         <v>0</v>
       </c>
       <c r="J220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">

</xml_diff>

<commit_message>
Site updated: 2024-08-07 21:23:23
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7954,22 +7954,22 @@
         <v>0</v>
       </c>
       <c r="E221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I221" t="n">
         <v>0</v>
       </c>
       <c r="J221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">

</xml_diff>

<commit_message>
Site updated: 2024-08-09 20:45:27
</commit_message>
<xml_diff>
--- a/statistics/2024_data.xlsx
+++ b/statistics/2024_data.xlsx
@@ -7982,28 +7982,28 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D222" t="n">
         <v>0</v>
       </c>
       <c r="E222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I222" t="n">
         <v>0</v>
       </c>
       <c r="J222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -8016,16 +8016,16 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D223" t="n">
         <v>0</v>
       </c>
       <c r="E223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G223" t="n">
         <v>0</v>
@@ -8037,7 +8037,7 @@
         <v>0</v>
       </c>
       <c r="J223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224">

</xml_diff>